<commit_message>
Dados para o conflito de capacidade
</commit_message>
<xml_diff>
--- a/Files/data/Testando Conflitos.xlsx
+++ b/Files/data/Testando Conflitos.xlsx
@@ -8,26 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDExt\GitHub\9Semestre\timetabling-UENF\Files\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA39278-7BDF-44C2-B25B-88D012377EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75621BF8-7253-4D96-B9D8-BBD37FDB60A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="1" xr2:uid="{459AFEA8-9D2F-404C-845E-545F3C50EB73}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="4" xr2:uid="{459AFEA8-9D2F-404C-845E-545F3C50EB73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sala" sheetId="2" r:id="rId1"/>
     <sheet name="Aluno" sheetId="3" r:id="rId2"/>
     <sheet name="Professor" sheetId="1" r:id="rId3"/>
+    <sheet name="Demandas" sheetId="4" r:id="rId4"/>
+    <sheet name="Capacidades" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="45">
   <si>
     <t>SEG</t>
   </si>
@@ -93,13 +104,82 @@
   </si>
   <si>
     <t>C, E, F</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>]},</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>mix</t>
+  </si>
+  <si>
+    <t>INF01112</t>
+  </si>
+  <si>
+    <t>INF01113</t>
+  </si>
+  <si>
+    <t>INF01114</t>
+  </si>
+  <si>
+    <t>INF01115</t>
+  </si>
+  <si>
+    <t>Alunos</t>
+  </si>
+  <si>
+    <t>Turmas</t>
+  </si>
+  <si>
+    <t>: { "cursando": [</t>
+  </si>
+  <si>
+    <t>Demanda</t>
+  </si>
+  <si>
+    <t>idturma</t>
+  </si>
+  <si>
+    <t>disciplinas</t>
+  </si>
+  <si>
+    <t>SALAS</t>
+  </si>
+  <si>
+    <t>CAPACIDADES</t>
+  </si>
+  <si>
+    <t>Disciplina</t>
+  </si>
+  <si>
+    <t>Sala do Horário 1</t>
+  </si>
+  <si>
+    <t>Sala do Horário 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,13 +187,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -137,6 +249,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F65A32-5CCB-4C97-8643-F922A31969C3}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -925,4 +1043,2200 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDB826E-F419-49B4-AF6F-A6CE69D2F56F}">
+  <dimension ref="A1:Q33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CHAR(34)&amp;A2&amp;CHAR(34)</f>
+        <v>"1"</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(B2,CHAR(34)&amp;B$1&amp;CHAR(34)&amp;IF(COUNTBLANK(K2:M2)=3,"",", "),"")</f>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K2" t="str">
+        <f>IF(C2,CHAR(34)&amp;C$1&amp;CHAR(34)&amp;IF(COUNTBLANK(L2:M2)=2,"",", "),"")</f>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(D2,CHAR(34)&amp;D$1&amp;CHAR(34)&amp;IF(COUNTBLANK(M2)=1,"",", "),"")</f>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(E2,CHAR(34)&amp;E$1&amp;CHAR(34),"")</f>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H17" si="0">CHAR(34)&amp;A3&amp;CHAR(34)</f>
+        <v>"2"</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J22" si="1">IF(B3,CHAR(34)&amp;B$1&amp;CHAR(34)&amp;IF(COUNTBLANK(K3:M3)=3,"",", "),"")</f>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K22" si="2">IF(C3,CHAR(34)&amp;C$1&amp;CHAR(34)&amp;IF(COUNTBLANK(L3:M3)=2,"",", "),"")</f>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L22" si="3">IF(D3,CHAR(34)&amp;D$1&amp;CHAR(34)&amp;IF(COUNTBLANK(M3)=1,"",", "),"")</f>
+        <v>"INF01114"</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M22" si="4">IF(E3,CHAR(34)&amp;E$1&amp;CHAR(34),"")</f>
+        <v/>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>"3"</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>"4"</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="2"/>
+        <v>"INF01113"</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>"5"</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>"6"</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="3"/>
+        <v>"INF01114"</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>"7"</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>"8"</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>"INF01112"</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>"9"</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>"10"</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="3"/>
+        <v>"INF01114"</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>"11"</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>"12"</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="2"/>
+        <v>"INF01113"</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>"13"</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>"14"</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="3"/>
+        <v>"INF01114"</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>"15"</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>"16"</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" ref="H19:H22" si="5">CHAR(34)&amp;A19&amp;CHAR(34)</f>
+        <v>"17"</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="5"/>
+        <v>"18"</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="5"/>
+        <v>"19"</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="5"/>
+        <v>"20"</v>
+      </c>
+      <c r="I22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0CB15C-BD37-4356-B3C7-0C01201858E9}">
+  <dimension ref="A1:Y33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" customWidth="1"/>
+    <col min="25" max="25" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CHAR(34)&amp;A2&amp;CHAR(34)</f>
+        <v>"1"</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(B2,CHAR(34)&amp;B$1&amp;CHAR(34)&amp;IF(COUNTBLANK(K2:M2)=3,"",", "),"")</f>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K2" t="str">
+        <f>IF(C2,CHAR(34)&amp;C$1&amp;CHAR(34)&amp;IF(COUNTBLANK(L2:M2)=2,"",", "),"")</f>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(D2,CHAR(34)&amp;D$1&amp;CHAR(34)&amp;IF(COUNTBLANK(M2)=1,"",", "),"")</f>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(E2,CHAR(34)&amp;E$1&amp;CHAR(34),"")</f>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2">
+        <v>9</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H17" si="0">CHAR(34)&amp;A3&amp;CHAR(34)</f>
+        <v>"2"</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J22" si="1">IF(B3,CHAR(34)&amp;B$1&amp;CHAR(34)&amp;IF(COUNTBLANK(K3:M3)=3,"",", "),"")</f>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K22" si="2">IF(C3,CHAR(34)&amp;C$1&amp;CHAR(34)&amp;IF(COUNTBLANK(L3:M3)=2,"",", "),"")</f>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L22" si="3">IF(D3,CHAR(34)&amp;D$1&amp;CHAR(34)&amp;IF(COUNTBLANK(M3)=1,"",", "),"")</f>
+        <v>"INF01114"</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M22" si="4">IF(E3,CHAR(34)&amp;E$1&amp;CHAR(34),"")</f>
+        <v/>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>"3"</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4">
+        <v>11</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>"4"</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="2"/>
+        <v>"INF01113"</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5">
+        <v>12</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>"5"</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>"6"</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="3"/>
+        <v>"INF01114"</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>"7"</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N8" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>"8"</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>"INF01112"</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>"9"</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>"10"</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="3"/>
+        <v>"INF01114"</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>"11"</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>"12"</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="2"/>
+        <v>"INF01113"</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>"13"</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>"14"</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="3"/>
+        <v>"INF01114"</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>"15"</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>"16"</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" ref="H19:H22" si="5">CHAR(34)&amp;A19&amp;CHAR(34)</f>
+        <v>"17"</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"INF01112", </v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="5"/>
+        <v>"18"</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"INF01113", </v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="5"/>
+        <v>"19"</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">"INF01114", </v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="5"/>
+        <v>"20"</v>
+      </c>
+      <c r="I22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="4"/>
+        <v>"INF01115"</v>
+      </c>
+      <c r="N22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Reavaliando distribuição de salas e turmas
</commit_message>
<xml_diff>
--- a/Files/data/Testando Conflitos.xlsx
+++ b/Files/data/Testando Conflitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDExt\GitHub\9Semestre\timetabling-UENF\Files\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75621BF8-7253-4D96-B9D8-BBD37FDB60A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C7C23F-85C3-4878-AF33-E0C27791A46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="4" xr2:uid="{459AFEA8-9D2F-404C-845E-545F3C50EB73}"/>
   </bookViews>
@@ -24,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="41">
   <si>
     <t>SEG</t>
   </si>
@@ -104,18 +95,6 @@
   </si>
   <si>
     <t>C, E, F</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
   </si>
   <si>
     <t>]},</t>
@@ -196,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,18 +194,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -240,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -253,8 +220,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1068,25 +1033,25 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1110,7 +1075,7 @@
         <v>"1"</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J2" t="str">
         <f>IF(B2,CHAR(34)&amp;B$1&amp;CHAR(34)&amp;IF(COUNTBLANK(K2:M2)=3,"",", "),"")</f>
@@ -1129,10 +1094,10 @@
         <v>"INF01115"</v>
       </c>
       <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -1159,7 +1124,7 @@
         <v>"2"</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J22" si="1">IF(B3,CHAR(34)&amp;B$1&amp;CHAR(34)&amp;IF(COUNTBLANK(K3:M3)=3,"",", "),"")</f>
@@ -1178,10 +1143,10 @@
         <v/>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q3">
         <v>2</v>
@@ -1208,7 +1173,7 @@
         <v>"3"</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="1"/>
@@ -1227,10 +1192,10 @@
         <v>"INF01115"</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -1257,7 +1222,7 @@
         <v>"4"</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="1"/>
@@ -1276,10 +1241,10 @@
         <v/>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1306,7 +1271,7 @@
         <v>"5"</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="1"/>
@@ -1325,7 +1290,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -1349,7 +1314,7 @@
         <v>"6"</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="1"/>
@@ -1368,7 +1333,7 @@
         <v/>
       </c>
       <c r="N7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1392,7 +1357,7 @@
         <v>"7"</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="1"/>
@@ -1411,7 +1376,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1435,7 +1400,7 @@
         <v>"8"</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="1"/>
@@ -1454,7 +1419,7 @@
         <v/>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1478,7 +1443,7 @@
         <v>"9"</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="1"/>
@@ -1497,7 +1462,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1521,7 +1486,7 @@
         <v>"10"</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="1"/>
@@ -1540,7 +1505,7 @@
         <v/>
       </c>
       <c r="N11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -1564,7 +1529,7 @@
         <v>"11"</v>
       </c>
       <c r="I12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="1"/>
@@ -1583,7 +1548,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1607,7 +1572,7 @@
         <v>"12"</v>
       </c>
       <c r="I13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="1"/>
@@ -1626,7 +1591,7 @@
         <v/>
       </c>
       <c r="N13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -1650,7 +1615,7 @@
         <v>"13"</v>
       </c>
       <c r="I14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="1"/>
@@ -1669,7 +1634,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -1693,7 +1658,7 @@
         <v>"14"</v>
       </c>
       <c r="I15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="1"/>
@@ -1712,7 +1677,7 @@
         <v/>
       </c>
       <c r="N15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -1736,7 +1701,7 @@
         <v>"15"</v>
       </c>
       <c r="I16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="1"/>
@@ -1755,7 +1720,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1779,7 +1744,7 @@
         <v>"16"</v>
       </c>
       <c r="I17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="1"/>
@@ -1798,7 +1763,7 @@
         <v/>
       </c>
       <c r="N17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1808,7 +1773,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="1"/>
@@ -1848,7 +1813,7 @@
         <v>"17"</v>
       </c>
       <c r="I19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="1"/>
@@ -1867,7 +1832,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -1889,7 +1854,7 @@
         <v>"18"</v>
       </c>
       <c r="I20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="1"/>
@@ -1908,7 +1873,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -1928,7 +1893,7 @@
         <v>"19"</v>
       </c>
       <c r="I21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="1"/>
@@ -1947,7 +1912,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -1965,7 +1930,7 @@
         <v>"20"</v>
       </c>
       <c r="I22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="1"/>
@@ -1984,7 +1949,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1994,7 +1959,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="G23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -2078,7 +2043,7 @@
   <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2104,49 +2069,49 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" t="s">
         <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
@@ -2170,7 +2135,7 @@
         <v>"1"</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J2" t="str">
         <f>IF(B2,CHAR(34)&amp;B$1&amp;CHAR(34)&amp;IF(COUNTBLANK(K2:M2)=3,"",", "),"")</f>
@@ -2189,13 +2154,13 @@
         <v>"INF01115"</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="O2">
         <v>9</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -2204,19 +2169,19 @@
         <v>1</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="U2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="X2" s="6" t="s">
+      <c r="V2" t="s">
         <v>13</v>
       </c>
+      <c r="X2" t="s">
+        <v>13</v>
+      </c>
       <c r="Y2">
-        <v>9</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
@@ -2240,7 +2205,7 @@
         <v>"2"</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J22" si="1">IF(B3,CHAR(34)&amp;B$1&amp;CHAR(34)&amp;IF(COUNTBLANK(K3:M3)=3,"",", "),"")</f>
@@ -2259,13 +2224,13 @@
         <v/>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="O3">
         <v>10</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q3">
         <v>2</v>
@@ -2274,19 +2239,19 @@
         <v>2</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" t="s">
         <v>14</v>
       </c>
+      <c r="V3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X3" t="s">
+        <v>14</v>
+      </c>
       <c r="Y3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
@@ -2310,7 +2275,7 @@
         <v>"3"</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="1"/>
@@ -2329,13 +2294,13 @@
         <v>"INF01115"</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="O4">
         <v>11</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -2344,19 +2309,19 @@
         <v>3</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="X4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4" t="s">
         <v>15</v>
       </c>
+      <c r="V4" t="s">
+        <v>13</v>
+      </c>
+      <c r="X4" t="s">
+        <v>15</v>
+      </c>
       <c r="Y4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
@@ -2380,7 +2345,7 @@
         <v>"4"</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="1"/>
@@ -2399,13 +2364,13 @@
         <v/>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="O5">
         <v>12</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -2414,19 +2379,13 @@
         <v>4</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y5">
-        <v>99</v>
+        <v>28</v>
+      </c>
+      <c r="U5" t="s">
+        <v>15</v>
+      </c>
+      <c r="V5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
@@ -2450,7 +2409,7 @@
         <v>"5"</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="1"/>
@@ -2469,13 +2428,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y6">
-        <v>99</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
@@ -2499,7 +2452,7 @@
         <v>"6"</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="1"/>
@@ -2518,13 +2471,7 @@
         <v/>
       </c>
       <c r="N7" t="s">
-        <v>26</v>
-      </c>
-      <c r="X7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y7">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
@@ -2548,7 +2495,7 @@
         <v>"7"</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="1"/>
@@ -2567,13 +2514,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N8" t="s">
-        <v>26</v>
-      </c>
-      <c r="X8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y8">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
@@ -2597,7 +2538,7 @@
         <v>"8"</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="1"/>
@@ -2616,13 +2557,7 @@
         <v/>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y9">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
@@ -2646,7 +2581,7 @@
         <v>"9"</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="1"/>
@@ -2665,7 +2600,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
@@ -2689,7 +2624,7 @@
         <v>"10"</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="1"/>
@@ -2708,7 +2643,7 @@
         <v/>
       </c>
       <c r="N11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
@@ -2732,7 +2667,7 @@
         <v>"11"</v>
       </c>
       <c r="I12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="1"/>
@@ -2751,7 +2686,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
@@ -2775,7 +2710,7 @@
         <v>"12"</v>
       </c>
       <c r="I13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="1"/>
@@ -2794,7 +2729,7 @@
         <v/>
       </c>
       <c r="N13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
@@ -2818,7 +2753,7 @@
         <v>"13"</v>
       </c>
       <c r="I14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="1"/>
@@ -2837,7 +2772,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
@@ -2861,7 +2796,7 @@
         <v>"14"</v>
       </c>
       <c r="I15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="1"/>
@@ -2880,7 +2815,7 @@
         <v/>
       </c>
       <c r="N15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
@@ -2904,7 +2839,7 @@
         <v>"15"</v>
       </c>
       <c r="I16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="1"/>
@@ -2923,7 +2858,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -2947,7 +2882,7 @@
         <v>"16"</v>
       </c>
       <c r="I17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="1"/>
@@ -2966,7 +2901,7 @@
         <v/>
       </c>
       <c r="N17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -2976,7 +2911,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="1"/>
@@ -3016,7 +2951,7 @@
         <v>"17"</v>
       </c>
       <c r="I19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="1"/>
@@ -3035,7 +2970,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -3057,7 +2992,7 @@
         <v>"18"</v>
       </c>
       <c r="I20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="1"/>
@@ -3076,7 +3011,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -3096,7 +3031,7 @@
         <v>"19"</v>
       </c>
       <c r="I21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="1"/>
@@ -3115,7 +3050,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -3133,7 +3068,7 @@
         <v>"20"</v>
       </c>
       <c r="I22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="1"/>
@@ -3152,7 +3087,7 @@
         <v>"INF01115"</v>
       </c>
       <c r="N22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -3162,7 +3097,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="G23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Conflitos de capacidades de turma
</commit_message>
<xml_diff>
--- a/Files/data/Testando Conflitos.xlsx
+++ b/Files/data/Testando Conflitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDExt\GitHub\9Semestre\timetabling-UENF\Files\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C7C23F-85C3-4878-AF33-E0C27791A46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3113EFC-2919-431D-B5C7-2C4C53F6FA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="4" xr2:uid="{459AFEA8-9D2F-404C-845E-545F3C50EB73}"/>
   </bookViews>
@@ -24,12 +24,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="41">
   <si>
     <t>SEG</t>
   </si>
@@ -175,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +203,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -207,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -218,6 +251,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2043,7 +2088,7 @@
   <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2159,16 +2204,16 @@
       <c r="O2">
         <v>9</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="U2" t="s">
@@ -2181,7 +2226,7 @@
         <v>13</v>
       </c>
       <c r="Y2">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
@@ -2229,23 +2274,23 @@
       <c r="O3">
         <v>10</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="Q3">
         <v>2</v>
       </c>
       <c r="S3">
-        <v>2</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="U3" t="s">
         <v>14</v>
       </c>
       <c r="V3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="X3" t="s">
         <v>14</v>
@@ -2299,23 +2344,23 @@
       <c r="O4">
         <v>11</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="8" t="s">
         <v>28</v>
       </c>
       <c r="Q4">
         <v>1</v>
       </c>
       <c r="S4">
-        <v>3</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="U4" t="s">
         <v>15</v>
       </c>
       <c r="V4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="X4" t="s">
         <v>15</v>
@@ -2369,20 +2414,20 @@
       <c r="O5">
         <v>12</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="9" t="s">
         <v>29</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S5">
-        <v>4</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>28</v>
+        <v>2</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="U5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V5" t="s">
         <v>13</v>
@@ -2430,6 +2475,18 @@
       <c r="N6" t="s">
         <v>22</v>
       </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
@@ -2473,6 +2530,18 @@
       <c r="N7" t="s">
         <v>22</v>
       </c>
+      <c r="S7">
+        <v>4</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U7" t="s">
+        <v>15</v>
+      </c>
+      <c r="V7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
@@ -2516,6 +2585,18 @@
       <c r="N8" t="s">
         <v>22</v>
       </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="U8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
@@ -2558,6 +2639,18 @@
       </c>
       <c r="N9" t="s">
         <v>22</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="U9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">

</xml_diff>